<commit_message>
Heatmap improved, marketCap added, correlation and decomposition, gridsearch
</commit_message>
<xml_diff>
--- a/Market_cap_09aug.xlsx
+++ b/Market_cap_09aug.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>OSSRu</t>
   </si>
@@ -89,18 +89,67 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Percentage of total</t>
+    <t>TICKER</t>
+  </si>
+  <si>
+    <t>Market Cap 
+in Million Isk</t>
+  </si>
+  <si>
+    <t>Market Cap 
+in £ Million</t>
+  </si>
+  <si>
+    <t>Percentage
+ of total</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Telecoms</t>
+  </si>
+  <si>
+    <t>Food Processing</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Fishing</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>IT and Tech</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +172,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,12 +189,117 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -146,11 +308,74 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -467,242 +692,545 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="7"/>
+    <col min="4" max="4" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2">
+      <c r="J1" s="2">
         <f>SUM(B2:B18)</f>
         <v>1014557201014</v>
       </c>
-      <c r="H1" s="3">
-        <f>G1/$G$1</f>
+      <c r="K1" s="3">
+        <f>J1/$J$1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="M1" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>264145118855</v>
       </c>
-      <c r="C2" s="3">
-        <f>B2/$G$1</f>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="12">
+        <f>ROUND(B2,-6)/$M$1</f>
+        <v>264145</v>
+      </c>
+      <c r="F2" s="12">
+        <f>+E2/$M$2</f>
+        <v>1886.75</v>
+      </c>
+      <c r="G2" s="23">
+        <f>B2/$J$1</f>
         <v>0.26035507765456689</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="15"/>
+      <c r="M2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>196723226250</v>
       </c>
-      <c r="C3" s="3">
-        <f>B3/$G$1</f>
+      <c r="C3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="12">
+        <f>ROUND(B3,-6)/$M$1</f>
+        <v>196723</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F19" si="0">+E3/$M$2</f>
+        <v>1405.1642857142858</v>
+      </c>
+      <c r="G3" s="23">
+        <f>B3/$J$1</f>
         <v>0.19390057657999452</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>69115435325</v>
       </c>
-      <c r="C4" s="3">
-        <f>B4/$G$1</f>
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <f>ROUND(B4,-6)/$M$1</f>
+        <v>69115</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" si="0"/>
+        <v>493.67857142857144</v>
+      </c>
+      <c r="G4" s="23">
+        <f>B4/$J$1</f>
         <v>6.8123744285608065E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>69019668000</v>
       </c>
-      <c r="C5" s="3">
-        <f>B5/$G$1</f>
+      <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="12">
+        <f>ROUND(B5,-6)/$M$1</f>
+        <v>69020</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>493</v>
+      </c>
+      <c r="G5" s="23">
+        <f>B5/$J$1</f>
         <v>6.8029351061742238E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>58581176753</v>
       </c>
-      <c r="C6" s="3">
-        <f>B6/$G$1</f>
+      <c r="C6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="12">
+        <f>ROUND(B6,-6)/$M$1</f>
+        <v>58581</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>418.43571428571431</v>
+      </c>
+      <c r="G6" s="23">
+        <f>B6/$J$1</f>
         <v>5.7740634726608807E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
         <v>58231439760</v>
       </c>
-      <c r="C7" s="3">
-        <f>B7/$G$1</f>
+      <c r="C7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12">
+        <f>ROUND(B7,-6)/$M$1</f>
+        <v>58231</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="0"/>
+        <v>415.93571428571431</v>
+      </c>
+      <c r="G7" s="23">
+        <f>B7/$J$1</f>
         <v>5.7395915875221762E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>42348268657</v>
       </c>
-      <c r="C8" s="3">
-        <f>B8/$G$1</f>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="12">
+        <f>ROUND(B8,-6)/$M$1</f>
+        <v>42348</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="0"/>
+        <v>302.48571428571427</v>
+      </c>
+      <c r="G8" s="23">
+        <f>B8/$J$1</f>
         <v>4.1740641744669488E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>40671095000</v>
       </c>
-      <c r="C9" s="3">
-        <f>B9/$G$1</f>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="12">
+        <f>ROUND(B9,-6)/$M$1</f>
+        <v>40671</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="0"/>
+        <v>290.50714285714287</v>
+      </c>
+      <c r="G9" s="23">
+        <f>B9/$J$1</f>
         <v>4.0087532727924299E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>38237453825</v>
       </c>
-      <c r="C10" s="3">
-        <f>B10/$G$1</f>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12">
+        <f>ROUND(B10,-6)/$M$1</f>
+        <v>38237</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>273.12142857142857</v>
+      </c>
+      <c r="G10" s="23">
+        <f>B10/$J$1</f>
         <v>3.768881023838138E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>36983270655</v>
       </c>
-      <c r="C11" s="3">
-        <f>B11/$G$1</f>
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="12">
+        <f>ROUND(B11,-6)/$M$1</f>
+        <v>36983</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>264.16428571428571</v>
+      </c>
+      <c r="G11" s="23">
+        <f>B11/$J$1</f>
         <v>3.6452622501754503E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1">
         <v>28125000000</v>
       </c>
-      <c r="C12" s="3">
-        <f>B12/$G$1</f>
+      <c r="C12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="12">
+        <f>ROUND(B12,-6)/$M$1</f>
+        <v>28125</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>200.89285714285714</v>
+      </c>
+      <c r="G12" s="23">
+        <f>B12/$J$1</f>
         <v>2.7721453232888639E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>26073349649</v>
       </c>
-      <c r="C13" s="3">
-        <f>B13/$G$1</f>
+      <c r="C13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="12">
+        <f>ROUND(B13,-6)/$M$1</f>
+        <v>26073</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>186.23571428571429</v>
+      </c>
+      <c r="G13" s="23">
+        <f>B13/$J$1</f>
         <v>2.5699240637138025E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>22234975410</v>
       </c>
-      <c r="C14" s="3">
-        <f>B14/$G$1</f>
+      <c r="C14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="12">
+        <f>ROUND(B14,-6)/$M$1</f>
+        <v>22235</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>158.82142857142858</v>
+      </c>
+      <c r="G14" s="23">
+        <f>B14/$J$1</f>
         <v>2.1915940656453116E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1">
         <v>21497122607</v>
       </c>
-      <c r="C15" s="3">
-        <f>B15/$G$1</f>
+      <c r="C15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="12">
+        <f>ROUND(B15,-6)/$M$1</f>
+        <v>21497</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>153.55000000000001</v>
+      </c>
+      <c r="G15" s="23">
+        <f>B15/$J$1</f>
         <v>2.1188674808591063E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>16847061304</v>
       </c>
-      <c r="C16" s="3">
-        <f>B16/$G$1</f>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="12">
+        <f>ROUND(B16,-6)/$M$1</f>
+        <v>16847</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>120.33571428571429</v>
+      </c>
+      <c r="G16" s="23">
+        <f>B16/$J$1</f>
         <v>1.6605334117349116E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1">
         <v>14490774617</v>
       </c>
-      <c r="C17" s="3">
-        <f>B17/$G$1</f>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="12">
+        <f>ROUND(B17,-6)/$M$1</f>
+        <v>14491</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>103.50714285714285</v>
+      </c>
+      <c r="G17" s="23">
+        <f>B17/$J$1</f>
         <v>1.4282856208124277E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>11232764347</v>
       </c>
-      <c r="C18" s="3">
-        <f>B18/$G$1</f>
+      <c r="C18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="13">
+        <f>ROUND(B18,-6)/$M$1</f>
+        <v>11233</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="0"/>
+        <v>80.23571428571428</v>
+      </c>
+      <c r="G18" s="24">
+        <f>B18/$J$1</f>
         <v>1.10715929429838E-2</v>
+      </c>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="21">
+        <f>SUM(B2:B18)</f>
+        <v>1014557201014</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="21">
+        <f>SUM(E2:E18)</f>
+        <v>1014555</v>
+      </c>
+      <c r="F19" s="20">
+        <f>SUM(F2:F18)</f>
+        <v>7246.8214285714294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="21">
+        <v>1000000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>